<commit_message>
converting to wide format of TS (data.table::cast)
</commit_message>
<xml_diff>
--- a/data/source/TS_supplemental.xlsx
+++ b/data/source/TS_supplemental.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8916"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t>studyid</t>
   </si>
@@ -74,9 +74,6 @@
     <t>C100762</t>
   </si>
   <si>
-    <t>siteid_im</t>
-  </si>
-  <si>
     <t>NOTES</t>
   </si>
   <si>
@@ -101,12 +98,6 @@
     <t>ISO8601</t>
   </si>
   <si>
-    <t>adminact_im</t>
-  </si>
-  <si>
-    <t>arm_im</t>
-  </si>
-  <si>
     <t>Pbo</t>
   </si>
   <si>
@@ -179,10 +170,22 @@
     <t>blindedtreatment</t>
   </si>
   <si>
-    <t>epoch_im</t>
-  </si>
-  <si>
     <t>Epoch Blinded treatment</t>
+  </si>
+  <si>
+    <t>siteid</t>
+  </si>
+  <si>
+    <t>adminact</t>
+  </si>
+  <si>
+    <t>arm</t>
+  </si>
+  <si>
+    <t>epoch</t>
+  </si>
+  <si>
+    <t>DO NOT USE UNDERBARS in any TSPARMCD values. Due to later CAST function from long to wide.</t>
   </si>
 </sst>
 </file>
@@ -549,24 +552,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -595,27 +598,27 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="N1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="O1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
@@ -629,10 +632,13 @@
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -650,195 +656,195 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2">
         <v>701</v>
       </c>
       <c r="O4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" t="s">
         <v>31</v>
       </c>
-      <c r="K6" t="s">
-        <v>34</v>
-      </c>
       <c r="L6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
       </c>
       <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" t="s">
         <v>39</v>
       </c>
-      <c r="K8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" t="s">
-        <v>42</v>
-      </c>
       <c r="N8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="N9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>44</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" t="s">
         <v>48</v>
-      </c>
-      <c r="G10" t="s">
-        <v>50</v>
-      </c>
-      <c r="L10" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip prior to merge to get AO's latest data.
</commit_message>
<xml_diff>
--- a/data/source/TS_supplemental.xlsx
+++ b/data/source/TS_supplemental.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
   <si>
     <t>studyid</t>
   </si>
@@ -83,15 +83,6 @@
     <t>DataCutoff</t>
   </si>
   <si>
-    <t>preflbl_im</t>
-  </si>
-  <si>
-    <t>lbl_im</t>
-  </si>
-  <si>
-    <t>type_im</t>
-  </si>
-  <si>
     <t>Data cutoff admin activity. Label should be the value of dcutdesc in the TS domain</t>
   </si>
   <si>
@@ -101,30 +92,15 @@
     <t>Pbo</t>
   </si>
   <si>
-    <t>ScreenFailure</t>
-  </si>
-  <si>
-    <t>XanolemineHigh</t>
-  </si>
-  <si>
-    <t>XanolemineLow</t>
-  </si>
-  <si>
     <t>ControlArm</t>
   </si>
   <si>
     <t>FalseArm</t>
   </si>
   <si>
-    <t>type2_im</t>
-  </si>
-  <si>
     <t>RandomizationOutcome</t>
   </si>
   <si>
-    <t>altlbl_im</t>
-  </si>
-  <si>
     <t>Placebo</t>
   </si>
   <si>
@@ -167,9 +143,6 @@
     <t>Epoch Blinded Treatment</t>
   </si>
   <si>
-    <t>blindedtreatment</t>
-  </si>
-  <si>
     <t>Epoch Blinded treatment</t>
   </si>
   <si>
@@ -186,6 +159,84 @@
   </si>
   <si>
     <t>DO NOT USE UNDERBARS in any TSPARMCD values. Due to later CAST function from long to wide.</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>type2</t>
+  </si>
+  <si>
+    <t>visit</t>
+  </si>
+  <si>
+    <t>AmbulECGPlace</t>
+  </si>
+  <si>
+    <t>AmbulECGRemove</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Retrieval</t>
+  </si>
+  <si>
+    <t>Screening1</t>
+  </si>
+  <si>
+    <t>Screening2</t>
+  </si>
+  <si>
+    <t>Wk12</t>
+  </si>
+  <si>
+    <t>wk16</t>
+  </si>
+  <si>
+    <t>wk20</t>
+  </si>
+  <si>
+    <t>wk24</t>
+  </si>
+  <si>
+    <t>wk26</t>
+  </si>
+  <si>
+    <t>wk2</t>
+  </si>
+  <si>
+    <t>wk4</t>
+  </si>
+  <si>
+    <t>wk6</t>
+  </si>
+  <si>
+    <t>wk8</t>
+  </si>
+  <si>
+    <t>Wk16</t>
+  </si>
+  <si>
+    <t>Wk20</t>
+  </si>
+  <si>
+    <t>Wk24</t>
+  </si>
+  <si>
+    <t>Wk2</t>
+  </si>
+  <si>
+    <t>Wk26</t>
+  </si>
+  <si>
+    <t>Wk4</t>
+  </si>
+  <si>
+    <t>Wk6</t>
+  </si>
+  <si>
+    <t>Wk8</t>
   </si>
 </sst>
 </file>
@@ -201,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +262,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,6 +299,10 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,10 +633,9 @@
     <col min="7" max="7" width="23.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -598,27 +664,18 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
@@ -632,13 +689,13 @@
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -656,195 +713,423 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2">
         <v>701</v>
       </c>
-      <c r="O4" t="s">
+      <c r="L4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
       </c>
       <c r="J7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L7" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J8" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="K8" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" t="s">
-        <v>39</v>
-      </c>
-      <c r="N8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="K9" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" t="s">
-        <v>40</v>
-      </c>
-      <c r="N9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="4">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="4">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
         <v>52</v>
       </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" t="s">
-        <v>48</v>
+      <c r="G15" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="4">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="4">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="4">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="4">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="4">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="4">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="4">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="4">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="4">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="4">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start conversion of AE
</commit_message>
<xml_diff>
--- a/data/source/TS_supplemental.xlsx
+++ b/data/source/TS_supplemental.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
   <si>
     <t>studyid</t>
   </si>
@@ -65,12 +65,6 @@
     <t>Primary Outcome Measure</t>
   </si>
   <si>
-    <t>ADAS-cog</t>
-  </si>
-  <si>
-    <t>Evaluate the efficacy and safety of transdermal xanomeline, 50cm2 and 75cm2, and placebo in subjects with mild to moderate Alzheimers disease.</t>
-  </si>
-  <si>
     <t>C100762</t>
   </si>
   <si>
@@ -188,30 +182,6 @@
     <t>Wk12</t>
   </si>
   <si>
-    <t>wk16</t>
-  </si>
-  <si>
-    <t>wk20</t>
-  </si>
-  <si>
-    <t>wk24</t>
-  </si>
-  <si>
-    <t>wk26</t>
-  </si>
-  <si>
-    <t>wk2</t>
-  </si>
-  <si>
-    <t>wk4</t>
-  </si>
-  <si>
-    <t>wk6</t>
-  </si>
-  <si>
-    <t>wk8</t>
-  </si>
-  <si>
     <t>Wk16</t>
   </si>
   <si>
@@ -237,6 +207,30 @@
   </si>
   <si>
     <t>Xan_Lo</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>studytype</t>
+  </si>
+  <si>
+    <t>Study Type</t>
+  </si>
+  <si>
+    <t>Trial Phase</t>
+  </si>
+  <si>
+    <t>PHASE2</t>
+  </si>
+  <si>
+    <t>phase</t>
+  </si>
+  <si>
+    <t>ADAS-Cog</t>
+  </si>
+  <si>
+    <t>Evaluate the efficacy and safety of transdermal xanomeline, 50cm2 and 75cm2, and placebo in subjects with mild to moderate Alzheimer's disease.</t>
   </si>
 </sst>
 </file>
@@ -617,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:E21"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,18 +658,18 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
@@ -687,15 +681,15 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -707,429 +701,463 @@
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2">
         <v>701</v>
       </c>
       <c r="L4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s">
         <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="4">
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
       <c r="G12" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="4">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="4">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="4">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="4">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="4">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="G19" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="4">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="4">
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="G21" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="4">
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="G22" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B23" s="4">
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="G23" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="4">
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="G24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" s="4">
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>